<commit_message>
Ajout des appréciations pour le S1
</commit_message>
<xml_diff>
--- a/excel/M1-S1/M1-S1-MAGI.xlsx
+++ b/excel/M1-S1/M1-S1-MAGI.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndyVESPUCE\bulletin-espi\backend\excel\M1-S1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF96F646-D1A4-49C3-9167-9EDA8B1CB199}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{182A2ECD-C062-43BE-8135-6AB8DA7C6C74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="59610" yWindow="3390" windowWidth="21630" windowHeight="11250" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15270" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="32">
   <si>
     <t>UE 1 – Economie &amp; Gestion</t>
   </si>
@@ -118,6 +118,9 @@
   </si>
   <si>
     <t>CodeApprenant</t>
+  </si>
+  <si>
+    <t>AppreciationPeriode</t>
   </si>
 </sst>
 </file>
@@ -637,18 +640,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AD32"/>
+  <dimension ref="A1:AE32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AG8" sqref="AG8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="22" max="22" width="18.44140625" customWidth="1"/>
+    <col min="31" max="31" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
@@ -717,8 +721,9 @@
       <c r="AB1" s="3"/>
       <c r="AC1" s="3"/>
       <c r="AD1" s="3"/>
-    </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE1" s="3"/>
+    </row>
+    <row r="2" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>30</v>
       </c>
@@ -809,8 +814,11 @@
       <c r="AD2" s="8" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE2" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A3" s="9"/>
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
@@ -841,8 +849,9 @@
       <c r="AB3" s="12"/>
       <c r="AC3" s="10"/>
       <c r="AD3" s="12"/>
-    </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE3" s="12"/>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A4" s="13"/>
       <c r="B4" s="13"/>
       <c r="C4" s="13"/>
@@ -873,8 +882,9 @@
       <c r="AB4" s="15"/>
       <c r="AC4" s="14"/>
       <c r="AD4" s="15"/>
-    </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE4" s="15"/>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
       <c r="B5" s="16"/>
       <c r="C5" s="16"/>
@@ -905,8 +915,9 @@
       <c r="AB5" s="12"/>
       <c r="AC5" s="17"/>
       <c r="AD5" s="12"/>
-    </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE5" s="12"/>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A6" s="13"/>
       <c r="B6" s="13"/>
       <c r="C6" s="13"/>
@@ -937,8 +948,9 @@
       <c r="AB6" s="15"/>
       <c r="AC6" s="14"/>
       <c r="AD6" s="15"/>
-    </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE6" s="15"/>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A7" s="16"/>
       <c r="B7" s="16"/>
       <c r="C7" s="16"/>
@@ -969,8 +981,9 @@
       <c r="AB7" s="12"/>
       <c r="AC7" s="17"/>
       <c r="AD7" s="12"/>
-    </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE7" s="12"/>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A8" s="13"/>
       <c r="B8" s="13"/>
       <c r="C8" s="13"/>
@@ -1001,8 +1014,9 @@
       <c r="AB8" s="15"/>
       <c r="AC8" s="14"/>
       <c r="AD8" s="15"/>
-    </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE8" s="15"/>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A9" s="16"/>
       <c r="B9" s="16"/>
       <c r="C9" s="16"/>
@@ -1033,8 +1047,9 @@
       <c r="AB9" s="12"/>
       <c r="AC9" s="17"/>
       <c r="AD9" s="12"/>
-    </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE9" s="12"/>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A10" s="13"/>
       <c r="B10" s="13"/>
       <c r="C10" s="13"/>
@@ -1065,8 +1080,9 @@
       <c r="AB10" s="15"/>
       <c r="AC10" s="14"/>
       <c r="AD10" s="15"/>
-    </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE10" s="15"/>
+    </row>
+    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A11" s="16"/>
       <c r="B11" s="16"/>
       <c r="C11" s="16"/>
@@ -1097,8 +1113,9 @@
       <c r="AB11" s="12"/>
       <c r="AC11" s="17"/>
       <c r="AD11" s="12"/>
-    </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE11" s="12"/>
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A12" s="13"/>
       <c r="B12" s="13"/>
       <c r="C12" s="13"/>
@@ -1129,8 +1146,9 @@
       <c r="AB12" s="15"/>
       <c r="AC12" s="14"/>
       <c r="AD12" s="15"/>
-    </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE12" s="15"/>
+    </row>
+    <row r="13" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A13" s="16"/>
       <c r="B13" s="16"/>
       <c r="C13" s="16"/>
@@ -1161,8 +1179,9 @@
       <c r="AB13" s="12"/>
       <c r="AC13" s="17"/>
       <c r="AD13" s="12"/>
-    </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE13" s="12"/>
+    </row>
+    <row r="14" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A14" s="13"/>
       <c r="B14" s="13"/>
       <c r="C14" s="13"/>
@@ -1193,8 +1212,9 @@
       <c r="AB14" s="15"/>
       <c r="AC14" s="14"/>
       <c r="AD14" s="15"/>
-    </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE14" s="15"/>
+    </row>
+    <row r="15" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A15" s="16"/>
       <c r="B15" s="16"/>
       <c r="C15" s="16"/>
@@ -1225,8 +1245,9 @@
       <c r="AB15" s="12"/>
       <c r="AC15" s="17"/>
       <c r="AD15" s="12"/>
-    </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE15" s="12"/>
+    </row>
+    <row r="16" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A16" s="13"/>
       <c r="B16" s="13"/>
       <c r="C16" s="13"/>
@@ -1257,8 +1278,9 @@
       <c r="AB16" s="15"/>
       <c r="AC16" s="14"/>
       <c r="AD16" s="15"/>
-    </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE16" s="15"/>
+    </row>
+    <row r="17" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A17" s="16"/>
       <c r="B17" s="16"/>
       <c r="C17" s="16"/>
@@ -1289,8 +1311,9 @@
       <c r="AB17" s="12"/>
       <c r="AC17" s="17"/>
       <c r="AD17" s="12"/>
-    </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE17" s="12"/>
+    </row>
+    <row r="18" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A18" s="13"/>
       <c r="B18" s="13"/>
       <c r="C18" s="13"/>
@@ -1321,8 +1344,9 @@
       <c r="AB18" s="15"/>
       <c r="AC18" s="14"/>
       <c r="AD18" s="15"/>
-    </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE18" s="15"/>
+    </row>
+    <row r="19" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A19" s="16"/>
       <c r="B19" s="16"/>
       <c r="C19" s="16"/>
@@ -1353,8 +1377,9 @@
       <c r="AB19" s="12"/>
       <c r="AC19" s="17"/>
       <c r="AD19" s="12"/>
-    </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE19" s="12"/>
+    </row>
+    <row r="20" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A20" s="13"/>
       <c r="B20" s="13"/>
       <c r="C20" s="13"/>
@@ -1385,8 +1410,9 @@
       <c r="AB20" s="15"/>
       <c r="AC20" s="14"/>
       <c r="AD20" s="15"/>
-    </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE20" s="15"/>
+    </row>
+    <row r="21" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A21" s="16"/>
       <c r="B21" s="16"/>
       <c r="C21" s="16"/>
@@ -1417,8 +1443,9 @@
       <c r="AB21" s="12"/>
       <c r="AC21" s="17"/>
       <c r="AD21" s="12"/>
-    </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE21" s="12"/>
+    </row>
+    <row r="22" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A22" s="13"/>
       <c r="B22" s="13"/>
       <c r="C22" s="13"/>
@@ -1449,8 +1476,9 @@
       <c r="AB22" s="15"/>
       <c r="AC22" s="14"/>
       <c r="AD22" s="15"/>
-    </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE22" s="15"/>
+    </row>
+    <row r="23" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A23" s="16"/>
       <c r="B23" s="16"/>
       <c r="C23" s="16"/>
@@ -1481,8 +1509,9 @@
       <c r="AB23" s="12"/>
       <c r="AC23" s="17"/>
       <c r="AD23" s="12"/>
-    </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE23" s="12"/>
+    </row>
+    <row r="24" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A24" s="13"/>
       <c r="B24" s="13"/>
       <c r="C24" s="13"/>
@@ -1513,8 +1542,9 @@
       <c r="AB24" s="15"/>
       <c r="AC24" s="14"/>
       <c r="AD24" s="15"/>
-    </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE24" s="15"/>
+    </row>
+    <row r="25" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A25" s="16"/>
       <c r="B25" s="16"/>
       <c r="C25" s="16"/>
@@ -1545,8 +1575,9 @@
       <c r="AB25" s="12"/>
       <c r="AC25" s="17"/>
       <c r="AD25" s="12"/>
-    </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE25" s="12"/>
+    </row>
+    <row r="26" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A26" s="13"/>
       <c r="B26" s="13"/>
       <c r="C26" s="13"/>
@@ -1577,8 +1608,9 @@
       <c r="AB26" s="15"/>
       <c r="AC26" s="14"/>
       <c r="AD26" s="15"/>
-    </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE26" s="15"/>
+    </row>
+    <row r="27" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A27" s="16"/>
       <c r="B27" s="16"/>
       <c r="C27" s="16"/>
@@ -1609,8 +1641,9 @@
       <c r="AB27" s="12"/>
       <c r="AC27" s="17"/>
       <c r="AD27" s="12"/>
-    </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE27" s="12"/>
+    </row>
+    <row r="28" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A28" s="13"/>
       <c r="B28" s="13"/>
       <c r="C28" s="13"/>
@@ -1641,8 +1674,9 @@
       <c r="AB28" s="15"/>
       <c r="AC28" s="14"/>
       <c r="AD28" s="15"/>
-    </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE28" s="15"/>
+    </row>
+    <row r="29" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A29" s="16"/>
       <c r="B29" s="16"/>
       <c r="C29" s="16"/>
@@ -1673,8 +1707,9 @@
       <c r="AB29" s="12"/>
       <c r="AC29" s="17"/>
       <c r="AD29" s="12"/>
-    </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE29" s="12"/>
+    </row>
+    <row r="30" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A30" s="13"/>
       <c r="B30" s="13"/>
       <c r="C30" s="13"/>
@@ -1705,8 +1740,9 @@
       <c r="AB30" s="15"/>
       <c r="AC30" s="14"/>
       <c r="AD30" s="15"/>
-    </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE30" s="15"/>
+    </row>
+    <row r="31" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A31" s="16"/>
       <c r="B31" s="16"/>
       <c r="C31" s="16"/>
@@ -1737,8 +1773,9 @@
       <c r="AB31" s="12"/>
       <c r="AC31" s="17"/>
       <c r="AD31" s="12"/>
-    </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE31" s="12"/>
+    </row>
+    <row r="32" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A32" s="13"/>
       <c r="B32" s="13"/>
       <c r="C32" s="13"/>
@@ -1769,6 +1806,7 @@
       <c r="AB32" s="15"/>
       <c r="AC32" s="14"/>
       <c r="AD32" s="15"/>
+      <c r="AE32" s="15"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:C2 A4:C4">

</xml_diff>

<commit_message>
Commit des appréciations M1S1, M1S2, M2S3, M2S4
</commit_message>
<xml_diff>
--- a/excel/M1-S1/M1-S1-MAGI.xlsx
+++ b/excel/M1-S1/M1-S1-MAGI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndyVESPUCE\bulletin-espi\backend\excel\M1-S1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{182A2ECD-C062-43BE-8135-6AB8DA7C6C74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA9DE8F3-CC29-49D8-8828-BA87CC8D5A42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15270" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33795" yWindow="1995" windowWidth="17280" windowHeight="8880" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -120,7 +120,7 @@
     <t>CodeApprenant</t>
   </si>
   <si>
-    <t>AppreciationPeriode</t>
+    <t>Appreciations</t>
   </si>
 </sst>
 </file>
@@ -642,8 +642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AG8" sqref="AG8"/>
+    <sheetView tabSelected="1" topLeftCell="T1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AE2" sqref="AE2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Mise en place de l'import des documents effectué
</commit_message>
<xml_diff>
--- a/excel/M1-S1/M1-S1-MAGI.xlsx
+++ b/excel/M1-S1/M1-S1-MAGI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndyVESPUCE\bulletin-espi\backend\excel\M1-S1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA9DE8F3-CC29-49D8-8828-BA87CC8D5A42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{504885BA-D5C6-470A-B6B9-75B134604651}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33795" yWindow="1995" windowWidth="17280" windowHeight="8880" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8880" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -642,8 +642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AE2" sqref="AE2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>